<commit_message>
Update data preparation, begin housing benefits analysis
</commit_message>
<xml_diff>
--- a/data/codebook.xlsx
+++ b/data/codebook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skvrnami/github/housinc-precarity/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC73457B-35E6-6A47-B624-C71EFAED1F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF71C365-5999-9940-8E72-5AA4EE2CB2BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{AEA44D95-819B-1C48-A562-66134390B6FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="101">
   <si>
     <t>original_variable_name</t>
   </si>
@@ -330,6 +330,15 @@
   </si>
   <si>
     <t>HS060</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Yes, for sole use of the household</t>
+  </si>
+  <si>
+    <t>Yes, shared</t>
   </si>
 </sst>
 </file>
@@ -702,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93AD84D8-A24B-E44E-BC69-1925E06E1F1C}">
-  <dimension ref="A1:D89"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -720,6 +729,9 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1042,7 +1054,7 @@
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1050,89 +1062,83 @@
         <v>2</v>
       </c>
       <c r="D35" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>46</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>47</v>
       </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38" t="s">
-        <v>49</v>
-      </c>
       <c r="C38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C39">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C40">
-        <v>3</v>
-      </c>
-      <c r="D40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>51</v>
-      </c>
-      <c r="B41" t="s">
-        <v>50</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D42" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B43" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -1151,10 +1157,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -1173,10 +1179,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B47" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -1195,10 +1201,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B49" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -1217,10 +1223,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -1239,16 +1245,16 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B53" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1256,287 +1262,287 @@
         <v>2</v>
       </c>
       <c r="D54" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>63</v>
+      </c>
+      <c r="B55" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C55">
-        <v>3</v>
-      </c>
-      <c r="D55" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>66</v>
-      </c>
-      <c r="B56" t="s">
-        <v>67</v>
-      </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
-      <c r="D56" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C57">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D57" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>66</v>
+      </c>
+      <c r="B58" t="s">
+        <v>67</v>
+      </c>
       <c r="C58">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C59">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D59" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C60">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D60" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>74</v>
-      </c>
-      <c r="B61" t="s">
-        <v>73</v>
-      </c>
       <c r="C61">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D61" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C62">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D62" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>74</v>
+      </c>
+      <c r="B63" t="s">
+        <v>73</v>
+      </c>
       <c r="C63">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C64">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D64" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>79</v>
-      </c>
-      <c r="B65" t="s">
-        <v>80</v>
-      </c>
       <c r="C65">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D65" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C66">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D66" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>79</v>
+      </c>
+      <c r="B67" t="s">
+        <v>80</v>
+      </c>
       <c r="C67">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C68">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D68" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>81</v>
-      </c>
-      <c r="B69" t="s">
-        <v>84</v>
-      </c>
       <c r="C69">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D69" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C70">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D70" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>81</v>
+      </c>
+      <c r="B71" t="s">
+        <v>84</v>
+      </c>
       <c r="C71">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D71" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C72">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D72" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>82</v>
-      </c>
-      <c r="B73" t="s">
-        <v>85</v>
-      </c>
       <c r="C73">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D73" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C74">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D74" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>82</v>
+      </c>
+      <c r="B75" t="s">
+        <v>85</v>
+      </c>
       <c r="C75">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D75" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C76">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D76" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>83</v>
-      </c>
-      <c r="B77" t="s">
-        <v>86</v>
-      </c>
       <c r="C77">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D77" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C78">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D78" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>83</v>
+      </c>
+      <c r="B79" t="s">
+        <v>86</v>
+      </c>
       <c r="C79">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D79" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C80">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D80" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>87</v>
-      </c>
-      <c r="B81" t="s">
-        <v>88</v>
-      </c>
       <c r="C81">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D81" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C82">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D82" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B83" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C83">
         <v>1</v>
       </c>
       <c r="D83" t="s">
-        <v>91</v>
+        <v>19</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -1544,52 +1550,74 @@
         <v>2</v>
       </c>
       <c r="D84" t="s">
-        <v>92</v>
+        <v>20</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>89</v>
+      </c>
+      <c r="B85" t="s">
+        <v>90</v>
+      </c>
       <c r="C85">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D85" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C86">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D86" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C87">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D87" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>97</v>
-      </c>
-      <c r="B88" t="s">
-        <v>96</v>
-      </c>
       <c r="C88">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D88" t="s">
-        <v>19</v>
+        <v>94</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C89">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D89" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>97</v>
+      </c>
+      <c r="B90" t="s">
+        <v>96</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+      <c r="D90" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C91">
+        <v>2</v>
+      </c>
+      <c r="D91" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>